<commit_message>
final updates to indicator code for WS_SRCE_P_IMP and FP_NADM_W_PDM
</commit_message>
<xml_diff>
--- a/Country_indicator_details_20160620_ProcessStatus.xlsx
+++ b/Country_indicator_details_20160620_ProcessStatus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\map-fs1.ndph.ox.ac.uk\map_data\DHS_Automation\Processing\DHS_Extractions_For_DHS\DHSmapping2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\map-fs1.ndph.ox.ac.uk\map_data\DHS_Automation\Processing\DHS_Extractions_For_DHS\DHSmapping2016_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -692,9 +692,6 @@
     <t>Calculated using married OR currently-living-with-partner (v501 = 1 OR v501 = 2)</t>
   </si>
   <si>
-    <t>Cannot get absolute values to match BUT proportions do match the API</t>
-  </si>
-  <si>
     <t>No response from API for Chad</t>
   </si>
   <si>
@@ -719,15 +716,9 @@
     <t>This is recorded in and can be calculated from either the household schedule level data or the individual (women) level data. Both should in theory give same results but do not. I've done the former as this duplicates the stata code. The selection of cases to include (denom and num) is quite complex! However none of the results match the totals in the API - although the percentages do now match. There IS data for cambodia but NOT for kenya, unlike shown here.</t>
   </si>
   <si>
-    <t>Calculated a result which matches closely not a precise match (e.g. percentage but not absolute), or have been unable to check</t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>Skipping - e.g. because it's non standard</t>
-  </si>
-  <si>
     <t>Need more work or failed</t>
   </si>
   <si>
@@ -738,6 +729,15 @@
   </si>
   <si>
     <t>Calculated using married OR currently-living-with-partner (v501 = 1 OR v501 = 2). Cannot get match for Kenya: note that denom should be the same as "using any modern method" but in the API the denom for Kenya (only) is different, so I think the API is wrong</t>
+  </si>
+  <si>
+    <t>Cannot get absolute values to match BUT proportions do match the API. This is because the API contains the "wrong" denominator values: the denominator in the API is correct for "something" but not for the indicator in question. Calculated values should be ok to use.</t>
+  </si>
+  <si>
+    <t>Skipping - e.g. because it's non standard. Don't use any result that's been calculated.</t>
+  </si>
+  <si>
+    <t>Calculated a result which matches closely not a precise match (e.g. percentage but not absolute), or have been unable to check. Should be ok to use with provisos.</t>
   </si>
 </sst>
 </file>
@@ -938,7 +938,7 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1020,9 +1020,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1629,8 +1626,8 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I9" sqref="I9"/>
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,39 +1733,39 @@
       <c r="C3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="39" t="s">
+      <c r="D3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="G3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="38"/>
+      <c r="G3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="37"/>
       <c r="N3" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="S3" s="46" t="s">
-        <v>201</v>
+      <c r="S3" s="45" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1781,45 +1778,45 @@
       <c r="C4" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="36"/>
+      <c r="D4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="44"/>
       <c r="N4" s="14" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="S4" s="44" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="106.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+      <c r="S4" s="43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>6</v>
       </c>
@@ -1829,39 +1826,39 @@
       <c r="C5" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M5" s="38"/>
+      <c r="D5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="37"/>
       <c r="N5" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="S5" s="41" t="s">
         <v>204</v>
+      </c>
+      <c r="S5" s="40" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1874,39 +1871,39 @@
       <c r="C6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="37" t="s">
         <v>37</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="J6" s="38" t="s">
+      <c r="J6" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="38" t="s">
+      <c r="K6" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="M6" s="42"/>
+      <c r="M6" s="41"/>
       <c r="N6" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="S6" s="43" t="s">
-        <v>203</v>
+        <v>194</v>
+      </c>
+      <c r="S6" s="42" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1919,39 +1916,39 @@
       <c r="C7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="E7" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="38" t="s">
+      <c r="F7" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="38" t="s">
+      <c r="J7" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="L7" s="38" t="s">
+      <c r="L7" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="M7" s="42"/>
+      <c r="M7" s="41"/>
       <c r="N7" s="14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
         <v>10</v>
       </c>
@@ -1961,36 +1958,36 @@
       <c r="C8" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="39" t="s">
+      <c r="D8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L8" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" s="38"/>
+      <c r="K8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M8" s="37"/>
       <c r="N8" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2003,39 +2000,39 @@
       <c r="C9" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" s="38"/>
+      <c r="D9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="37"/>
       <c r="N9" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
         <v>12</v>
       </c>
@@ -2045,36 +2042,36 @@
       <c r="C10" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M10" s="38"/>
+      <c r="D10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" s="37"/>
       <c r="N10" s="14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2090,31 +2087,31 @@
       <c r="D11" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="38" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M11" s="39"/>
+      <c r="G11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="38"/>
     </row>
     <row r="12" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
@@ -2129,33 +2126,33 @@
       <c r="D12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="38" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M12" s="40"/>
+      <c r="G12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="39"/>
       <c r="N12" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2168,34 +2165,34 @@
       <c r="C13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="38" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="M13" s="38"/>
+      <c r="F13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="37"/>
     </row>
     <row r="14" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
@@ -2207,34 +2204,34 @@
       <c r="C14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="L14" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M14" s="38"/>
+      <c r="D14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="37"/>
     </row>
     <row r="15" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
@@ -2255,30 +2252,30 @@
       <c r="F15" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="39" t="s">
+      <c r="G15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="38" t="s">
         <v>35</v>
       </c>
       <c r="L15" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="M15" s="41"/>
+      <c r="M15" s="40"/>
       <c r="N15" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="195.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="165.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>7</v>
       </c>
@@ -2291,33 +2288,33 @@
       <c r="D16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="45" t="s">
+      <c r="F16" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="44" t="s">
         <v>35</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="45" t="s">
+      <c r="I16" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="44" t="s">
         <v>35</v>
       </c>
       <c r="K16" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="L16" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="41"/>
+      <c r="L16" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="40"/>
       <c r="N16" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -2330,36 +2327,36 @@
       <c r="C17" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="I17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="L17" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="M17" s="44"/>
+      <c r="D17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="43"/>
       <c r="N17" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>